<commit_message>
add query parameter in creatLeaveReport API
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,53 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15" count="15">
-  <x:si>
-    <x:t>_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>isActive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>employeeDetails</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leavedetails</x:t>
-  </x:si>
-  <x:si>
-    <x:t>employeeOfficeDetails</x:t>
-  </x:si>
-  <x:si>
-    <x:t>month</x:t>
-  </x:si>
-  <x:si>
-    <x:t>year</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leave_type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leaveTypeName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leaveStatus</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"_id":2,"userName":"1010002","fullName":"Test Group HR Head 2","profileImage":"profile/963388b8.hydrangeas.jpg"}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"_id":1,"updatedAt":"2018-08-17T05:26:15.665Z","createdAt":"2018-06-24T08:38:43.999Z","leave_type":1,"createdBy":8,"updatedBy":2,"attachment":"externalDocument/a42d4cd4.api list-2.pdf","status":"Pending Withdrawal","reason":"Rejected","days":2,"toDate":"2018-08-14T07:53:16.000Z","fromDate":"2018-08-12T08:53:16.000Z","createdByName":{"_id":8,"fullName":"Akshay k"},"updatedByName":{"_id":2,"fullName":"Test Group HR Head 2"},"supervisorDetails":[{"_id":5,"fullName":"Reviewer 5"}]}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"_id":2,"emp_id":2,"departments":{"_id":1,"departmentName":"International Business"},"divisions":{"_id":1,"divisionName":"Business"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Annual Leave</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pending Withdrawal</x:t>
-  </x:si>
-</x:sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,70 +375,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="J1" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="A2" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="n">
-        <x:v>2018</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="1" spans="1:0"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>